<commit_message>
Day3 of N8N learning
</commit_message>
<xml_diff>
--- a/n8n-Journal.xlsx
+++ b/n8n-Journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -50,16 +50,26 @@
   </si>
   <si>
     <t xml:space="preserve">Meal &amp; Health Planner.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GitHub Push Email Notifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sends an email when a new push happens in my GitHub repo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n8n_workflow_notifier.json</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -134,7 +144,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,6 +158,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -168,13 +182,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -224,6 +238,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="n">
+        <v>45904</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Day4 of N8N learning
</commit_message>
<xml_diff>
--- a/n8n-Journal.xlsx
+++ b/n8n-Journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -59,16 +59,26 @@
   </si>
   <si>
     <t xml:space="preserve">n8n_workflow_notifier.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mood playlisty fetcher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fetches spotify playlist based on mood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mood_chnager.json</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -143,7 +153,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,6 +167,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -177,13 +191,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -247,6 +261,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="n">
+        <v>45905</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Day 5 of N8N Learning
</commit_message>
<xml_diff>
--- a/n8n-Journal.xlsx
+++ b/n8n-Journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t xml:space="preserve">mood_chnager.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citizen Complaint Response Automation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automates Typeform submissions by checking age eligibility and sending personalized Gmail responses based on complaint type.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citizen Complaint Response Automation.json</t>
   </si>
 </sst>
 </file>
@@ -191,13 +200,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -262,7 +271,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="3" t="n">
         <v>45905</v>
       </c>
       <c r="B5" s="0" t="s">
@@ -273,6 +282,20 @@
       </c>
       <c r="D5" s="0" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 6 of N8N Learning
</commit_message>
<xml_diff>
--- a/n8n-Journal.xlsx
+++ b/n8n-Journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t xml:space="preserve">Citizen Complaint Response Automation.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-Powered Complaint Chatbot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chatbot that uses Gemini Pro to handle citizen complaints with smart replies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI-Powered Complaint Chatbot.json</t>
   </si>
 </sst>
 </file>
@@ -200,13 +209,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -285,8 +294,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="n">
-        <v>45916</v>
+      <c r="A6" s="3" t="n">
+        <v>45915</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>16</v>
@@ -296,6 +305,20 @@
       </c>
       <c r="D6" s="0" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="n">
+        <v>45916</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 7 of N8N Learning
</commit_message>
<xml_diff>
--- a/n8n-Journal.xlsx
+++ b/n8n-Journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t xml:space="preserve">AI-Powered Complaint Chatbot.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complaint Intelligence Router</t>
+  </si>
+  <si>
+    <t xml:space="preserve">: Logs theft complaints via Gemini Pro with age-based eligibility and Google Sheets integration.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complaint Intelligence Router.json</t>
   </si>
 </sst>
 </file>
@@ -98,7 +107,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -127,6 +136,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -189,6 +204,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,13 +228,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.73046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -308,7 +327,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="3" t="n">
         <v>45916</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -319,6 +338,20 @@
       </c>
       <c r="D7" s="0" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="n">
+        <v>45917</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 8 of N8N Learning
</commit_message>
<xml_diff>
--- a/n8n-Journal.xlsx
+++ b/n8n-Journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t xml:space="preserve">Complaint Intelligence Router.json</t>
+  </si>
+  <si>
+    <t xml:space="preserve">today i updated the workflow to send assault report to sart team</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
     <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -136,12 +139,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -203,11 +200,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,13 +225,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -341,7 +338,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="3" t="n">
         <v>45917</v>
       </c>
       <c r="B8" s="0" t="s">
@@ -350,8 +347,22 @@
       <c r="C8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>45919</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Day 9 of N8N Learning
</commit_message>
<xml_diff>
--- a/n8n-Journal.xlsx
+++ b/n8n-Journal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t xml:space="preserve">today i updated the workflow to send assault report to sart team</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citizen Complaint Response Automation final</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Citizen Complaint Response Automation final.json</t>
   </si>
 </sst>
 </file>
@@ -225,13 +231,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -352,7 +358,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="3" t="n">
         <v>45919</v>
       </c>
       <c r="B9" s="0" t="s">
@@ -363,6 +369,20 @@
       </c>
       <c r="D9" s="0" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>45920</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>